<commit_message>
Get fixed QPSK values
</commit_message>
<xml_diff>
--- a/ps3/prob3/snr.xlsx
+++ b/ps3/prob3/snr.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="176" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="611" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,6 +38,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -122,7 +123,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -150,7 +151,7 @@
         <v>0.012</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>0.073</v>
+        <v>0.0254</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -161,7 +162,7 @@
         <v>0.012</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>0.061</v>
+        <v>0.0183</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -172,7 +173,7 @@
         <v>0.007</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>0.049</v>
+        <v>0.0118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -183,7 +184,7 @@
         <v>0.0028</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>0.035</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -194,7 +195,7 @@
         <v>0.0007</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.021</v>
+        <v>0.0022</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,7 +207,7 @@
         <v>9.60625E-005</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>0.011</v>
+        <v>0.0005</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -217,7 +218,8 @@
         <v>0</v>
       </c>
       <c r="C8" s="0" t="n">
-        <v>0.0007</v>
+        <f aca="false">4/16000000</f>
+        <v>2.5E-007</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,8 +230,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="0" t="n">
-        <f aca="false">18/16000000</f>
-        <v>1.125E-006</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>